<commit_message>
Data update. Model updates
</commit_message>
<xml_diff>
--- a/data/Cam_ElectionOffice.xlsx
+++ b/data/Cam_ElectionOffice.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet sheetId="1" r:id="rId1" name="Cam_ElectionOffice"/>
   </sheets>
+  <definedNames>
+    <definedName name="Cam_ElectionOffice">'Cam_ElectionOffice'!$A$1:$E$44</definedName>
+  </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
@@ -23,32 +26,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000" tint="0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000" tint="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000" tint="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000" tint="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000" tint="0"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -56,36 +33,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC0C0C0"/>
-        <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -96,80 +43,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD0D7E5"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFD0D7E5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD0D7E5"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD0D7E5"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD0D7E5"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFD0D7E5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD0D7E5"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD0D7E5"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD0D7E5"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFD0D7E5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD0D7E5"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD0D7E5"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyFill="1" applyProtection="1" applyAlignment="1" applyFont="1" xfId="0">
-      <alignment wrapText="0" vertical="center" horizontal="left"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
-      <alignment wrapText="0" vertical="center" horizontal="center"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
-      <alignment wrapText="0" vertical="center" horizontal="center"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
-      <alignment wrapText="1" vertical="center" horizontal="right"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
-      <alignment wrapText="1" vertical="center" horizontal="general"/>
-      <protection locked="1" hidden="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,813 +350,806 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col customWidth="true" min="1" max="1" width="14.0625"/>
-    <col customWidth="true" min="2" max="2" width="14.0625"/>
-    <col customWidth="true" min="3" max="3" width="14.0625"/>
-    <col customWidth="true" min="4" max="4" width="14.0625"/>
-    <col customWidth="true" min="5" max="5" width="14.0625"/>
-  </cols>
   <sheetData>
     <row outlineLevel="0" r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>ElectionOfficeId</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="0" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>StatusId</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="0" t="inlineStr">
         <is>
           <t>OfficeTypeId</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="0" t="inlineStr">
         <is>
           <t>Order</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="2">
-      <c r="A2" s="4">
+      <c r="A2" s="0">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>Tenth Judicial District</t>
         </is>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="C2" s="0">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0">
+        <v>3</v>
+      </c>
+      <c r="E2" s="0">
         <v>130</v>
       </c>
     </row>
     <row outlineLevel="0" r="3">
-      <c r="A3" s="4">
+      <c r="A3" s="0">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>Public Regulation Commissioner</t>
         </is>
       </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C3" s="0">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0">
         <v>4</v>
       </c>
     </row>
     <row outlineLevel="0" r="4">
-      <c r="A4" s="4">
+      <c r="A4" s="0">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>Justice Of The Supreme Court</t>
         </is>
       </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="C4" s="0">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0">
         <v>100</v>
       </c>
     </row>
     <row outlineLevel="0" r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="0">
         <v>15</v>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>Metropolitan Court Judge</t>
         </is>
       </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="C5" s="0">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0">
+        <v>3</v>
+      </c>
+      <c r="E5" s="0">
         <v>150</v>
       </c>
     </row>
     <row outlineLevel="0" r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="0">
         <v>16</v>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>Fourth Judicial District</t>
         </is>
       </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="C6" s="0">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0">
         <v>124</v>
       </c>
     </row>
     <row outlineLevel="0" r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="0">
         <v>17</v>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>Secretary Of State</t>
         </is>
       </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="C7" s="0">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0">
         <v>3</v>
       </c>
     </row>
     <row outlineLevel="0" r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="0">
         <v>18</v>
       </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>County Sheriff</t>
         </is>
       </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="0">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0">
         <v>6</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="0">
         <v>65</v>
       </c>
     </row>
     <row outlineLevel="0" r="9">
-      <c r="A9" s="4">
+      <c r="A9" s="0">
         <v>19</v>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>County Council</t>
         </is>
       </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C9" s="0">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0">
         <v>6</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="0">
         <v>64</v>
       </c>
     </row>
     <row outlineLevel="0" r="10">
-      <c r="A10" s="4">
+      <c r="A10" s="0">
         <v>20</v>
       </c>
-      <c r="B10" s="5" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>State Board Of Education</t>
         </is>
       </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="C10" s="0">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0">
         <v>8</v>
       </c>
     </row>
     <row outlineLevel="0" r="11">
-      <c r="A11" s="4">
+      <c r="A11" s="0">
         <v>21</v>
       </c>
-      <c r="B11" s="5" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>County Commissioner</t>
         </is>
       </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C11" s="0">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0">
         <v>6</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="0">
         <v>62</v>
       </c>
     </row>
     <row outlineLevel="0" r="12">
-      <c r="A12" s="4">
+      <c r="A12" s="0">
         <v>22</v>
       </c>
-      <c r="B12" s="5" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>Judge Of The Court Of Appeals - Retention</t>
         </is>
       </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
-        <v>3</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="C12" s="0">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0">
+        <v>3</v>
+      </c>
+      <c r="E12" s="0">
         <v>111</v>
       </c>
     </row>
     <row outlineLevel="0" r="13">
-      <c r="A13" s="4">
+      <c r="A13" s="0">
         <v>23</v>
       </c>
-      <c r="B13" s="5" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>State Senator</t>
         </is>
       </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4">
+      <c r="C13" s="0">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0">
         <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="14">
-      <c r="A14" s="4">
+      <c r="A14" s="0">
         <v>24</v>
       </c>
-      <c r="B14" s="5" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
         <is>
           <t>County Clerk</t>
         </is>
       </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14" s="0">
+        <v>1</v>
+      </c>
+      <c r="D14" s="0">
         <v>6</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="0">
         <v>61</v>
       </c>
     </row>
     <row outlineLevel="0" r="15">
-      <c r="A15" s="4">
+      <c r="A15" s="0">
         <v>25</v>
       </c>
-      <c r="B15" s="5" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
         <is>
           <t>Ninth Judicial District</t>
         </is>
       </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="C15" s="0">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0">
+        <v>3</v>
+      </c>
+      <c r="E15" s="0">
         <v>129</v>
       </c>
     </row>
     <row outlineLevel="0" r="16">
-      <c r="A16" s="4">
+      <c r="A16" s="0">
         <v>26</v>
       </c>
-      <c r="B16" s="5" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>Sixth Judicial District</t>
         </is>
       </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
-        <v>3</v>
-      </c>
-      <c r="E16" s="4">
+      <c r="C16" s="0">
+        <v>1</v>
+      </c>
+      <c r="D16" s="0">
+        <v>3</v>
+      </c>
+      <c r="E16" s="0">
         <v>126</v>
       </c>
     </row>
     <row outlineLevel="0" r="17">
-      <c r="A17" s="4">
+      <c r="A17" s="0">
         <v>27</v>
       </c>
-      <c r="B17" s="5" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>State Representative</t>
         </is>
       </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="C17" s="0">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0">
         <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="18">
-      <c r="A18" s="4">
+      <c r="A18" s="0">
         <v>28</v>
       </c>
-      <c r="B18" s="5" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr">
         <is>
           <t>County Assessor</t>
         </is>
       </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="C18" s="0">
+        <v>1</v>
+      </c>
+      <c r="D18" s="0">
         <v>6</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="0">
         <v>60</v>
       </c>
     </row>
     <row outlineLevel="0" r="19">
-      <c r="A19" s="4">
+      <c r="A19" s="0">
         <v>29</v>
       </c>
-      <c r="B19" s="5" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr">
         <is>
           <t>Second Judicial District</t>
         </is>
       </c>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4">
-        <v>3</v>
-      </c>
-      <c r="E19" s="4">
+      <c r="C19" s="0">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0">
+        <v>3</v>
+      </c>
+      <c r="E19" s="0">
         <v>122</v>
       </c>
     </row>
     <row outlineLevel="0" r="20">
-      <c r="A20" s="4">
+      <c r="A20" s="0">
         <v>30</v>
       </c>
-      <c r="B20" s="5" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr">
         <is>
           <t>County Treasurer</t>
         </is>
       </c>
-      <c r="C20" s="4">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="C20" s="0">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0">
         <v>6</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="0">
         <v>66</v>
       </c>
     </row>
     <row outlineLevel="0" r="21">
-      <c r="A21" s="4">
+      <c r="A21" s="0">
         <v>31</v>
       </c>
-      <c r="B21" s="5" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr">
         <is>
           <t>Probate Judge</t>
         </is>
       </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-      <c r="D21" s="4">
-        <v>3</v>
-      </c>
-      <c r="E21" s="4">
+      <c r="C21" s="0">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0">
+        <v>3</v>
+      </c>
+      <c r="E21" s="0">
         <v>160</v>
       </c>
     </row>
     <row outlineLevel="0" r="22">
-      <c r="A22" s="4">
+      <c r="A22" s="0">
         <v>32</v>
       </c>
-      <c r="B22" s="5" t="inlineStr">
+      <c r="B22" s="0" t="inlineStr">
         <is>
           <t>District Attorney</t>
         </is>
       </c>
-      <c r="C22" s="4">
-        <v>1</v>
-      </c>
-      <c r="D22" s="4">
-        <v>3</v>
-      </c>
-      <c r="E22" s="4">
+      <c r="C22" s="0">
+        <v>1</v>
+      </c>
+      <c r="D22" s="0">
+        <v>3</v>
+      </c>
+      <c r="E22" s="0">
         <v>170</v>
       </c>
     </row>
     <row outlineLevel="0" r="23">
-      <c r="A23" s="4">
+      <c r="A23" s="0">
         <v>33</v>
       </c>
-      <c r="B23" s="5" t="inlineStr">
+      <c r="B23" s="0" t="inlineStr">
         <is>
           <t>State Treasurer</t>
         </is>
       </c>
-      <c r="C23" s="4">
-        <v>1</v>
-      </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4">
+      <c r="C23" s="0">
+        <v>1</v>
+      </c>
+      <c r="D23" s="0">
+        <v>1</v>
+      </c>
+      <c r="E23" s="0">
         <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="24">
-      <c r="A24" s="4">
+      <c r="A24" s="0">
         <v>34</v>
       </c>
-      <c r="B24" s="5" t="inlineStr">
+      <c r="B24" s="0" t="inlineStr">
         <is>
           <t>Lieutenant Governor</t>
         </is>
       </c>
-      <c r="C24" s="4">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4">
-        <v>1</v>
-      </c>
-      <c r="E24" s="4">
+      <c r="C24" s="0">
+        <v>1</v>
+      </c>
+      <c r="D24" s="0">
+        <v>1</v>
+      </c>
+      <c r="E24" s="0">
         <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="25">
-      <c r="A25" s="4">
+      <c r="A25" s="0">
         <v>35</v>
       </c>
-      <c r="B25" s="5" t="inlineStr">
+      <c r="B25" s="0" t="inlineStr">
         <is>
           <t>Fifth Judicial District</t>
         </is>
       </c>
-      <c r="C25" s="4">
-        <v>1</v>
-      </c>
-      <c r="D25" s="4">
-        <v>3</v>
-      </c>
-      <c r="E25" s="4">
+      <c r="C25" s="0">
+        <v>1</v>
+      </c>
+      <c r="D25" s="0">
+        <v>3</v>
+      </c>
+      <c r="E25" s="0">
         <v>125</v>
       </c>
     </row>
     <row outlineLevel="0" r="26">
-      <c r="A26" s="4">
+      <c r="A26" s="0">
         <v>36</v>
       </c>
-      <c r="B26" s="5" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr">
         <is>
           <t>District Judge - Retention</t>
         </is>
       </c>
-      <c r="C26" s="4">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4">
-        <v>3</v>
-      </c>
-      <c r="E26" s="4">
+      <c r="C26" s="0">
+        <v>1</v>
+      </c>
+      <c r="D26" s="0">
+        <v>3</v>
+      </c>
+      <c r="E26" s="0">
         <v>181</v>
       </c>
     </row>
     <row outlineLevel="0" r="27">
-      <c r="A27" s="4">
+      <c r="A27" s="0">
         <v>37</v>
       </c>
-      <c r="B27" s="5" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr">
         <is>
           <t>Justice Of The Supreme Court - Retention</t>
         </is>
       </c>
-      <c r="C27" s="4">
-        <v>1</v>
-      </c>
-      <c r="D27" s="4">
-        <v>3</v>
-      </c>
-      <c r="E27" s="4">
+      <c r="C27" s="0">
+        <v>1</v>
+      </c>
+      <c r="D27" s="0">
+        <v>3</v>
+      </c>
+      <c r="E27" s="0">
         <v>101</v>
       </c>
     </row>
     <row outlineLevel="0" r="28">
-      <c r="A28" s="4">
+      <c r="A28" s="0">
         <v>38</v>
       </c>
-      <c r="B28" s="5" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr">
         <is>
           <t>Judge Of The Court Of Appeals</t>
         </is>
       </c>
-      <c r="C28" s="4">
-        <v>1</v>
-      </c>
-      <c r="D28" s="4">
-        <v>3</v>
-      </c>
-      <c r="E28" s="4">
+      <c r="C28" s="0">
+        <v>1</v>
+      </c>
+      <c r="D28" s="0">
+        <v>3</v>
+      </c>
+      <c r="E28" s="0">
         <v>110</v>
       </c>
     </row>
     <row outlineLevel="0" r="29">
-      <c r="A29" s="4">
+      <c r="A29" s="0">
         <v>39</v>
       </c>
-      <c r="B29" s="5" t="inlineStr">
+      <c r="B29" s="0" t="inlineStr">
         <is>
           <t>Governor Of New Mexico</t>
         </is>
       </c>
-      <c r="C29" s="4">
-        <v>1</v>
-      </c>
-      <c r="D29" s="4">
-        <v>1</v>
-      </c>
-      <c r="E29" s="4">
+      <c r="C29" s="0">
+        <v>1</v>
+      </c>
+      <c r="D29" s="0">
+        <v>1</v>
+      </c>
+      <c r="E29" s="0">
         <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="30">
-      <c r="A30" s="4">
+      <c r="A30" s="0">
         <v>40</v>
       </c>
-      <c r="B30" s="5" t="inlineStr">
+      <c r="B30" s="0" t="inlineStr">
         <is>
           <t>Municipal Judge</t>
         </is>
       </c>
-      <c r="C30" s="4">
-        <v>1</v>
-      </c>
-      <c r="D30" s="4">
-        <v>3</v>
-      </c>
-      <c r="E30" s="4">
+      <c r="C30" s="0">
+        <v>1</v>
+      </c>
+      <c r="D30" s="0">
+        <v>3</v>
+      </c>
+      <c r="E30" s="0">
         <v>190</v>
       </c>
     </row>
     <row outlineLevel="0" r="31">
-      <c r="A31" s="4">
+      <c r="A31" s="0">
         <v>41</v>
       </c>
-      <c r="B31" s="5" t="inlineStr">
+      <c r="B31" s="0" t="inlineStr">
         <is>
           <t>Public Education Commission</t>
         </is>
       </c>
-      <c r="C31" s="4">
-        <v>1</v>
-      </c>
-      <c r="D31" s="4">
+      <c r="C31" s="0">
+        <v>1</v>
+      </c>
+      <c r="D31" s="0">
         <v>5</v>
       </c>
     </row>
     <row outlineLevel="0" r="32">
-      <c r="A32" s="4">
+      <c r="A32" s="0">
         <v>42</v>
       </c>
-      <c r="B32" s="5" t="inlineStr">
+      <c r="B32" s="0" t="inlineStr">
         <is>
           <t>District Magistrate</t>
         </is>
       </c>
-      <c r="C32" s="4">
-        <v>1</v>
-      </c>
-      <c r="D32" s="4">
-        <v>3</v>
-      </c>
-      <c r="E32" s="4">
+      <c r="C32" s="0">
+        <v>1</v>
+      </c>
+      <c r="D32" s="0">
+        <v>3</v>
+      </c>
+      <c r="E32" s="0">
         <v>200</v>
       </c>
     </row>
     <row outlineLevel="0" r="33">
-      <c r="A33" s="4">
+      <c r="A33" s="0">
         <v>43</v>
       </c>
-      <c r="B33" s="5" t="inlineStr">
+      <c r="B33" s="0" t="inlineStr">
         <is>
           <t>Attorney General</t>
         </is>
       </c>
-      <c r="C33" s="4">
-        <v>1</v>
-      </c>
-      <c r="D33" s="4">
-        <v>1</v>
-      </c>
-      <c r="E33" s="4">
+      <c r="C33" s="0">
+        <v>1</v>
+      </c>
+      <c r="D33" s="0">
+        <v>1</v>
+      </c>
+      <c r="E33" s="0">
         <v>4</v>
       </c>
     </row>
     <row outlineLevel="0" r="34">
-      <c r="A34" s="4">
+      <c r="A34" s="0">
         <v>44</v>
       </c>
-      <c r="B34" s="5" t="inlineStr">
+      <c r="B34" s="0" t="inlineStr">
         <is>
           <t>County Surveyor</t>
         </is>
       </c>
-      <c r="C34" s="4">
-        <v>1</v>
-      </c>
-      <c r="D34" s="4">
+      <c r="C34" s="0">
+        <v>1</v>
+      </c>
+      <c r="D34" s="0">
         <v>6</v>
       </c>
     </row>
     <row outlineLevel="0" r="35">
-      <c r="A35" s="4">
+      <c r="A35" s="0">
         <v>45</v>
       </c>
-      <c r="B35" s="5" t="inlineStr">
+      <c r="B35" s="0" t="inlineStr">
         <is>
           <t>Corporation Commissioner</t>
         </is>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="0">
         <v>2</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="0">
         <v>4</v>
       </c>
     </row>
     <row outlineLevel="0" r="36">
-      <c r="A36" s="4">
+      <c r="A36" s="0">
         <v>46</v>
       </c>
-      <c r="B36" s="5" t="inlineStr">
+      <c r="B36" s="0" t="inlineStr">
         <is>
           <t>District Judge</t>
         </is>
       </c>
-      <c r="C36" s="4">
-        <v>1</v>
-      </c>
-      <c r="D36" s="4">
-        <v>3</v>
-      </c>
-      <c r="E36" s="4">
+      <c r="C36" s="0">
+        <v>1</v>
+      </c>
+      <c r="D36" s="0">
+        <v>3</v>
+      </c>
+      <c r="E36" s="0">
         <v>180</v>
       </c>
     </row>
     <row outlineLevel="0" r="37">
-      <c r="A37" s="4">
+      <c r="A37" s="0">
         <v>47</v>
       </c>
-      <c r="B37" s="5" t="inlineStr">
+      <c r="B37" s="0" t="inlineStr">
         <is>
           <t>State Auditor</t>
         </is>
       </c>
-      <c r="C37" s="4">
-        <v>1</v>
-      </c>
-      <c r="D37" s="4">
-        <v>1</v>
-      </c>
-      <c r="E37" s="4">
+      <c r="C37" s="0">
+        <v>1</v>
+      </c>
+      <c r="D37" s="0">
+        <v>1</v>
+      </c>
+      <c r="E37" s="0">
         <v>6</v>
       </c>
     </row>
     <row outlineLevel="0" r="38">
-      <c r="A38" s="4">
+      <c r="A38" s="0">
         <v>48</v>
       </c>
-      <c r="B38" s="5" t="inlineStr">
+      <c r="B38" s="0" t="inlineStr">
         <is>
           <t>Commissioner Of Public Lands</t>
         </is>
       </c>
-      <c r="C38" s="4">
-        <v>1</v>
-      </c>
-      <c r="D38" s="4">
-        <v>1</v>
-      </c>
-      <c r="E38" s="4">
+      <c r="C38" s="0">
+        <v>1</v>
+      </c>
+      <c r="D38" s="0">
+        <v>1</v>
+      </c>
+      <c r="E38" s="0">
         <v>7</v>
       </c>
     </row>
     <row outlineLevel="0" r="39">
-      <c r="A39" s="4">
+      <c r="A39" s="0">
         <v>49</v>
       </c>
-      <c r="B39" s="5" t="inlineStr">
+      <c r="B39" s="0" t="inlineStr">
         <is>
           <t>Magistrate Judge</t>
         </is>
       </c>
-      <c r="C39" s="4">
-        <v>1</v>
-      </c>
-      <c r="D39" s="4">
-        <v>3</v>
-      </c>
-      <c r="E39" s="4">
+      <c r="C39" s="0">
+        <v>1</v>
+      </c>
+      <c r="D39" s="0">
+        <v>3</v>
+      </c>
+      <c r="E39" s="0">
         <v>140</v>
       </c>
     </row>
     <row outlineLevel="0" r="40">
-      <c r="A40" s="4">
+      <c r="A40" s="0">
         <v>50</v>
       </c>
-      <c r="B40" s="5" t="inlineStr">
+      <c r="B40" s="0" t="inlineStr">
         <is>
           <t>Exploratory Campaign</t>
         </is>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="0">
         <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="41">
-      <c r="A41" s="4">
+      <c r="A41" s="0">
         <v>51</v>
       </c>
-      <c r="B41" s="5" t="inlineStr">
+      <c r="B41" s="0" t="inlineStr">
         <is>
           <t>Justice Of The Supreme Court - Voter Action Act</t>
         </is>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="0">
         <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="42">
-      <c r="A42" s="4">
+      <c r="A42" s="0">
         <v>52</v>
       </c>
-      <c r="B42" s="5" t="inlineStr">
+      <c r="B42" s="0" t="inlineStr">
         <is>
           <t>Judge Of The Court Of Appeals - Voter Action Act</t>
         </is>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="0">
         <v>2</v>
       </c>
     </row>
     <row outlineLevel="0" r="43">
-      <c r="A43" s="4">
+      <c r="A43" s="0">
         <v>53</v>
       </c>
-      <c r="B43" s="5" t="inlineStr">
+      <c r="B43" s="0" t="inlineStr">
         <is>
           <t>Public Regulation Commissioner - Voter Action Act</t>
         </is>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="0">
         <v>1</v>
       </c>
     </row>
     <row outlineLevel="0" r="44">
-      <c r="A44" s="4">
+      <c r="A44" s="0">
         <v>54</v>
       </c>
-      <c r="B44" s="5" t="inlineStr">
+      <c r="B44" s="0" t="inlineStr">
         <is>
           <t>School Board Member</t>
         </is>
       </c>
-      <c r="C44" s="4">
-        <v>1</v>
-      </c>
-      <c r="D44" s="4">
+      <c r="C44" s="0">
+        <v>1</v>
+      </c>
+      <c r="D44" s="0">
         <v>7</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="0">
         <v>700</v>
       </c>
     </row>

</xml_diff>